<commit_message>
first commit motor insurance
</commit_message>
<xml_diff>
--- a/bin/Debug/netcoreapp3.1/RequiredFiles/LoginNavigation.xlsx
+++ b/bin/Debug/netcoreapp3.1/RequiredFiles/LoginNavigation.xlsx
@@ -69,7 +69,7 @@
     <t>//*[contains(@class, 'mix Business --PolicyAdministration')]</t>
   </si>
   <si>
-    <t>//*[@id='password']</t>
+    <t>//*[@id="password"]</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>